<commit_message>
Basic work for fom builder and row editing.
</commit_message>
<xml_diff>
--- a/odk_app/config/tables/measure/forms/remeasure/remeasure.xlsx
+++ b/odk_app/config/tables/measure/forms/remeasure/remeasure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\dev\classes\capstone\app-designer-2.1.6\app\config\tables\measure\forms\remeasure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6066B78-C297-4184-8BE3-614A705CE2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDBEDB6-B89B-4DAA-A13B-DFD23FD78087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42210" yWindow="8265" windowWidth="21600" windowHeight="11505" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -784,9 +784,6 @@
     <t>measure</t>
   </si>
   <si>
-    <t>config/tables/measure/html/ingrowth_detail.html</t>
-  </si>
-  <si>
     <t>config/tables/measure/html/ingrowth_list.html</t>
   </si>
   <si>
@@ -794,6 +791,9 @@
   </si>
   <si>
     <t>unique to ingrowth</t>
+  </si>
+  <si>
+    <t>config/assets/form.html</t>
   </si>
 </sst>
 </file>
@@ -1391,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A68881D-8809-487D-A56B-3A7502CC8B35}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1448,7 +1448,7 @@
         <v>198</v>
       </c>
       <c r="E3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1465,7 +1465,7 @@
         <v>198</v>
       </c>
       <c r="E4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -1477,7 +1477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -2796,7 +2796,7 @@
         <v>198</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2807,7 +2807,7 @@
         <v>198</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Moved HTML files to their own folder.
</commit_message>
<xml_diff>
--- a/odk_app/config/tables/measure/forms/remeasure/remeasure.xlsx
+++ b/odk_app/config/tables/measure/forms/remeasure/remeasure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\dev\classes\capstone\app-designer-2.1.6\app\config\tables\measure\forms\remeasure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDBEDB6-B89B-4DAA-A13B-DFD23FD78087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE4D4BA-4322-40D8-A129-C115E05255D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5415" yWindow="6540" windowWidth="13080" windowHeight="15060" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -793,7 +793,7 @@
     <t>unique to ingrowth</t>
   </si>
   <si>
-    <t>config/assets/form.html</t>
+    <t>config/assets/html/form.html</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1392,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Simple search by tag for measure/mortality lists.
</commit_message>
<xml_diff>
--- a/odk_app/config/tables/measure/forms/remeasure/remeasure.xlsx
+++ b/odk_app/config/tables/measure/forms/remeasure/remeasure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\dev\classes\capstone\app-designer-2.1.6\app\config\tables\measure\forms\remeasure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE4D4BA-4322-40D8-A129-C115E05255D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E6F7B9-7EA9-48E7-A11D-EB36BC1D7D51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="6540" windowWidth="13080" windowHeight="15060" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9825" yWindow="4665" windowWidth="13080" windowHeight="15060" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -784,9 +784,6 @@
     <t>measure</t>
   </si>
   <si>
-    <t>config/tables/measure/html/ingrowth_list.html</t>
-  </si>
-  <si>
     <t>remeasure/ingrowth</t>
   </si>
   <si>
@@ -794,6 +791,9 @@
   </si>
   <si>
     <t>config/assets/html/form.html</t>
+  </si>
+  <si>
+    <t>config/assets/html/tree_record_list.html</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1392,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D13" sqref="D12:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1448,7 +1448,7 @@
         <v>198</v>
       </c>
       <c r="E3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1465,7 +1465,7 @@
         <v>198</v>
       </c>
       <c r="E4" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2796,7 +2796,7 @@
         <v>198</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2807,7 +2807,7 @@
         <v>198</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>